<commit_message>
ran match on new team respondents
</commit_message>
<xml_diff>
--- a/data/Team_Survey_Responses.xlsx
+++ b/data/Team_Survey_Responses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericberlow/Github/creative-landscape-survey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A151B73-3D68-7F42-ACCA-3433FA0797F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A6D991-AEA0-2A47-A180-2F87D28217F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3480" yWindow="-20040" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="team responses" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>#</t>
   </si>
@@ -212,13 +212,28 @@
   </si>
   <si>
     <t>Victor Ovcharov</t>
+  </si>
+  <si>
+    <t>dvbfimxrt3mpbsb8vhdvbfimxr4j0w2w</t>
+  </si>
+  <si>
+    <t>Vitaliy M</t>
+  </si>
+  <si>
+    <t>ovim7ribk0f7bp3i03ovimmzc043rj8x</t>
+  </si>
+  <si>
+    <t>Midday</t>
+  </si>
+  <si>
+    <t>Rodion Zhuvagin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -233,6 +248,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -256,12 +277,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,10 +602,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:AB15"/>
+      <selection activeCell="A17" sqref="A17:AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -593,7 +616,7 @@
     <col min="24" max="24" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -765,7 +788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -851,7 +874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -937,7 +960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -1023,7 +1046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -1109,7 +1132,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1195,7 +1218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -1281,7 +1304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1367,7 +1390,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1450,7 +1473,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1559,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1607,7 +1630,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
@@ -1695,7 +1718,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>60</v>
       </c>
@@ -1781,7 +1804,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -1865,6 +1888,181 @@
       </c>
       <c r="AB15" s="4" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>3</v>
+      </c>
+      <c r="I16" s="5">
+        <v>4</v>
+      </c>
+      <c r="J16" s="5">
+        <v>4</v>
+      </c>
+      <c r="K16" s="5">
+        <v>4</v>
+      </c>
+      <c r="L16" s="5">
+        <v>2</v>
+      </c>
+      <c r="M16" s="5">
+        <v>4</v>
+      </c>
+      <c r="N16" s="5">
+        <v>4</v>
+      </c>
+      <c r="O16" s="5">
+        <v>4</v>
+      </c>
+      <c r="P16" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>5</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" s="5">
+        <v>4</v>
+      </c>
+      <c r="T16" s="5">
+        <v>3</v>
+      </c>
+      <c r="U16" s="5">
+        <v>2</v>
+      </c>
+      <c r="V16" s="5">
+        <v>4</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="X16" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="5"/>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5">
+        <v>4</v>
+      </c>
+      <c r="I17" s="5">
+        <v>4</v>
+      </c>
+      <c r="J17" s="5">
+        <v>4</v>
+      </c>
+      <c r="K17" s="5">
+        <v>4</v>
+      </c>
+      <c r="L17" s="5">
+        <v>3</v>
+      </c>
+      <c r="M17" s="5">
+        <v>4</v>
+      </c>
+      <c r="N17" s="5">
+        <v>2</v>
+      </c>
+      <c r="O17" s="5">
+        <v>1</v>
+      </c>
+      <c r="P17" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>4</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="5">
+        <v>4</v>
+      </c>
+      <c r="T17" s="5">
+        <v>2</v>
+      </c>
+      <c r="U17" s="5">
+        <v>2</v>
+      </c>
+      <c r="V17" s="5">
+        <v>4</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA17" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>